<commit_message>
clean up AICUM survey
</commit_message>
<xml_diff>
--- a/preprocessing/data/AICUM Vaccination survey 1.19.2021.xlsx
+++ b/preprocessing/data/AICUM Vaccination survey 1.19.2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rob\AppData\Local\Packages\Microsoft.Office.Desktop_8wekyb3d8bbwe\AC\INetCache\Content.Outlook\K2IRH8X7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabe/Desktop/mggg/covid/covid-vaccines/preprocessing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C28B6912-AF3A-4C80-8D2E-4A8D2C6B7D36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F65BD0-D388-F445-AE1C-6BDFFBEEF950}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2C5482F3-50A0-4373-B3C3-CE59FB1944F4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{2C5482F3-50A0-4373-B3C3-CE59FB1944F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="109">
   <si>
     <t>Institution</t>
   </si>
@@ -216,9 +216,6 @@
     <t>Marisa Kelly</t>
   </si>
   <si>
-    <t>Umass Boston site</t>
-  </si>
-  <si>
     <t>Brandeis</t>
   </si>
   <si>
@@ -243,18 +240,12 @@
     <t>Kelsey DeVoe</t>
   </si>
   <si>
-    <t>Umass Medical School</t>
-  </si>
-  <si>
     <t>Williams</t>
   </si>
   <si>
     <t>Deborah Flynn</t>
   </si>
   <si>
-    <t>Southwester VT Medical Center and Berkshire Medical Center</t>
-  </si>
-  <si>
     <t>Wellesley</t>
   </si>
   <si>
@@ -312,9 +303,6 @@
     <t>soon</t>
   </si>
   <si>
-    <t>WP Clinic/community locations</t>
-  </si>
-  <si>
     <t>Smith</t>
   </si>
   <si>
@@ -352,6 +340,18 @@
   </si>
   <si>
     <t>Michael Jordan</t>
+  </si>
+  <si>
+    <t>UMass Boston</t>
+  </si>
+  <si>
+    <t>UMass Medical School</t>
+  </si>
+  <si>
+    <t>WP Clinic</t>
+  </si>
+  <si>
+    <t>Southwester VT Medical Center; Berkshire Medical Center</t>
   </si>
 </sst>
 </file>
@@ -714,27 +714,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DA02EF-295D-452B-857C-8FD03B17C6AF}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="1"/>
+    <col min="12" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -769,7 +769,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -795,7 +795,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -821,7 +821,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -850,7 +850,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -879,7 +879,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -911,7 +911,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -937,7 +937,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -969,7 +969,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -1049,9 +1049,6 @@
       <c r="F11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="H11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1059,7 +1056,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -1091,7 +1088,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
@@ -1117,7 +1114,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
@@ -1149,7 +1146,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
@@ -1181,7 +1178,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>53</v>
       </c>
@@ -1210,7 +1207,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>55</v>
       </c>
@@ -1236,7 +1233,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>57</v>
       </c>
@@ -1265,7 +1262,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>59</v>
       </c>
@@ -1291,7 +1288,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>61</v>
       </c>
@@ -1308,7 +1305,7 @@
         <v>13</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>22</v>
@@ -1323,12 +1320,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>12</v>
@@ -1352,12 +1349,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>12</v>
@@ -1384,38 +1381,38 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>12</v>
@@ -1430,7 +1427,7 @@
         <v>18</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>12</v>
@@ -1445,12 +1442,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>12</v>
@@ -1462,7 +1459,7 @@
         <v>13</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>75</v>
+        <v>108</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>13</v>
@@ -1477,12 +1474,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>12</v>
@@ -1509,12 +1506,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>12</v>
@@ -1526,7 +1523,7 @@
         <v>18</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>22</v>
@@ -1541,64 +1538,64 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>12</v>
@@ -1610,7 +1607,7 @@
         <v>18</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>13</v>
@@ -1622,12 +1619,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>12</v>
@@ -1651,12 +1648,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>13</v>
@@ -1680,12 +1677,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>12</v>
@@ -1694,13 +1691,13 @@
         <v>13</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>12</v>
@@ -1715,12 +1712,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>12</v>
@@ -1747,12 +1744,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>12</v>
@@ -1773,12 +1770,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>13</v>
@@ -1805,68 +1802,68 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="H38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="C39" s="1" t="s">
         <v>12</v>
       </c>
@@ -1877,7 +1874,7 @@
         <v>13</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>13</v>

</xml_diff>